<commit_message>
Time Slot Format Changed: 24 Hour to [0, 0, 0, 0, 0] (Array of states)
</commit_message>
<xml_diff>
--- a/algorithm/data/input.xlsx
+++ b/algorithm/data/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sessions" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="165">
   <si>
     <t xml:space="preserve">semester</t>
   </si>
@@ -327,9 +327,6 @@
     <t xml:space="preserve">10:00am-11:30am</t>
   </si>
   <si>
-    <t xml:space="preserve">9:30am-1:00pm</t>
-  </si>
-  <si>
     <t xml:space="preserve">HZ</t>
   </si>
   <si>
@@ -360,9 +357,6 @@
     <t xml:space="preserve">MJ</t>
   </si>
   <si>
-    <t xml:space="preserve">9:00am-1:00pm</t>
-  </si>
-  <si>
     <t xml:space="preserve">MMK</t>
   </si>
   <si>
@@ -375,19 +369,10 @@
     <t xml:space="preserve">SM</t>
   </si>
   <si>
-    <t xml:space="preserve">9:00am-1:00pm;2:00pm-5:00pm</t>
+    <t xml:space="preserve">8:30am-1:00pm;2:00pm-5:00pm</t>
   </si>
   <si>
     <t xml:space="preserve">MAI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8:30am-1:00pm;2:00pm-5:00pm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8:30am-10:00am</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8:00am-10:00pm;2:00pm-5:00pm</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -627,7 +612,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -668,6 +653,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,8 +676,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3311,8 +3300,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3441,7 +3430,7 @@
         <v>91</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>91</v>
@@ -3455,7 +3444,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>91</v>
@@ -3469,29 +3458,29 @@
         <v>93</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>93</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3499,19 +3488,19 @@
         <v>42</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>94</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,21 +3508,21 @@
         <v>65</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>94</v>
@@ -3553,10 +3542,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>93</v>
@@ -3573,19 +3562,19 @@
         <v>12</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3593,16 +3582,16 @@
         <v>40</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3610,13 +3599,13 @@
         <v>34</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>92</v>
@@ -3624,36 +3613,36 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>115</v>
-      </c>
       <c r="G19" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3679,47 +3668,49 @@
         <v>16</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>120</v>
+      <c r="C24" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3752,7 +3743,7 @@
   <dimension ref="A1:E1020"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3767,16 +3758,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E1" s="7"/>
     </row>
@@ -3785,13 +3776,13 @@
         <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E2" s="7"/>
     </row>
@@ -3800,13 +3791,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -3815,10 +3806,10 @@
         <v>96</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E4" s="7"/>
     </row>
@@ -3827,10 +3818,10 @@
         <v>98</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E5" s="7"/>
     </row>
@@ -3839,10 +3830,10 @@
         <v>99</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E6" s="7"/>
     </row>
@@ -3851,28 +3842,28 @@
         <v>59</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E8" s="7"/>
     </row>
@@ -3881,37 +3872,37 @@
         <v>36</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E11" s="7"/>
     </row>
@@ -3920,13 +3911,13 @@
         <v>42</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E12" s="7"/>
     </row>
@@ -3935,37 +3926,37 @@
         <v>65</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E15" s="7"/>
     </row>
@@ -3974,13 +3965,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E16" s="7"/>
     </row>
@@ -3989,13 +3980,13 @@
         <v>40</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E17" s="7"/>
     </row>
@@ -4004,43 +3995,43 @@
         <v>34</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="E18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E20" s="7"/>
     </row>
@@ -4049,13 +4040,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E21" s="7"/>
     </row>
@@ -4064,13 +4055,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E22" s="7"/>
     </row>
@@ -4079,13 +4070,13 @@
         <v>63</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="E23" s="7"/>
     </row>
@@ -4094,13 +4085,13 @@
         <v>14</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4108,10 +4099,10 @@
         <v>38</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
2 Session Per Week Routine - Working for the First Time
</commit_message>
<xml_diff>
--- a/algorithm/data/input.xlsx
+++ b/algorithm/data/input.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="165">
   <si>
     <t xml:space="preserve">semester</t>
   </si>
@@ -276,9 +276,6 @@
     <t xml:space="preserve">teacher</t>
   </si>
   <si>
-    <t xml:space="preserve">saturday</t>
-  </si>
-  <si>
     <t xml:space="preserve">sunday</t>
   </si>
   <si>
@@ -294,39 +291,45 @@
     <t xml:space="preserve">thursday</t>
   </si>
   <si>
-    <t xml:space="preserve">friday</t>
+    <t xml:space="preserve">10:00am-1:00pm;2:00pm-5:00pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:00pm-5:00pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:30am-1:00pm;2:00pm-5:00pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:00pm-3:30pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:30am-1:00pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:30am-1:00am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HHB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00am-11:30am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:30am-1:00pm;2:00pm-5:00pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00am-1:00pm;2:00pm-3:00pm</t>
   </si>
   <si>
     <t xml:space="preserve">10:00am-1:00pm</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00am-1:00pm;2:00pm-5:00pm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2:00pm-5:00pm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11:30am-1:00pm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2:00pm-3:30pm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MHA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8:30am-1:00am</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HHB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00am-11:30am</t>
-  </si>
-  <si>
     <t xml:space="preserve">HZ</t>
   </si>
   <si>
@@ -345,12 +348,12 @@
     <t xml:space="preserve">8:30am-11:30am; 2:00pm-5:00pm</t>
   </si>
   <si>
+    <t xml:space="preserve">8:30am-11:30am;11:30am-1:00pm;2:00pm-3:30pm</t>
+  </si>
+  <si>
     <t xml:space="preserve">8:30am-11:30am</t>
   </si>
   <si>
-    <t xml:space="preserve">11:30am-1:00pm;2:00pm-5:00pm</t>
-  </si>
-  <si>
     <t xml:space="preserve">AHK</t>
   </si>
   <si>
@@ -367,9 +370,6 @@
   </si>
   <si>
     <t xml:space="preserve">SM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8:30am-1:00pm;2:00pm-5:00pm</t>
   </si>
   <si>
     <t xml:space="preserve">MAI</t>
@@ -564,18 +564,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -612,7 +606,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -642,10 +636,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3298,23 +3288,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>83</v>
       </c>
@@ -3333,50 +3323,50 @@
       <c r="F1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B3" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="C3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>94</v>
@@ -3384,145 +3374,145 @@
       <c r="F4" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="6" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="D5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>59</v>
       </c>
+      <c r="B7" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="C7" s="6" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>102</v>
+      <c r="B9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="B12" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="C12" s="6" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>65</v>
       </c>
+      <c r="C13" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="D13" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>94</v>
@@ -3536,192 +3526,189 @@
       <c r="F14" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="6" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="B16" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="C16" s="6" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
         <v>40</v>
       </c>
+      <c r="C17" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="D17" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
         <v>34</v>
       </c>
+      <c r="B18" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="C18" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>91</v>
+        <v>101</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>102</v>
-      </c>
       <c r="E20" s="6" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="D21" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="E23" s="6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>91</v>
+      <c r="C25" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3746,7 +3733,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25"/>
@@ -3803,7 +3790,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>126</v>
@@ -3815,7 +3802,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>127</v>
@@ -3827,7 +3814,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>128</v>
@@ -3854,7 +3841,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>131</v>
@@ -3884,7 +3871,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>135</v>
@@ -3896,7 +3883,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>136</v>
@@ -3938,7 +3925,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>142</v>
@@ -3950,7 +3937,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>143</v>
@@ -4007,7 +3994,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>151</v>
@@ -4022,7 +4009,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
Resolved: Alternate Week Sesssion & No 2 Session of the Same Theory Course, On Same Day
</commit_message>
<xml_diff>
--- a/algorithm/data/input.xlsx
+++ b/algorithm/data/input.xlsx
@@ -3291,7 +3291,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3592,7 +3592,7 @@
         <v>101</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>89</v>

</xml_diff>